<commit_message>
Poda - borrador inicio
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>cap</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>Redundancia</t>
+  </si>
+  <si>
+    <t>Poda</t>
+  </si>
+  <si>
+    <t>borrador inicio</t>
+  </si>
+  <si>
+    <t>Espiritu</t>
   </si>
 </sst>
 </file>
@@ -69,12 +78,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,70 +92,64 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -165,14 +168,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -189,6 +184,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -204,6 +207,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -214,14 +224,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,187 +251,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,6 +493,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -529,162 +542,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1010,10 +1012,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1129,6 +1131,25 @@
         <v>7</v>
       </c>
     </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Idea general - borrador
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>cap</t>
   </si>
@@ -34,6 +34,12 @@
     <t>borrador parcial</t>
   </si>
   <si>
+    <t>Idea general</t>
+  </si>
+  <si>
+    <t>borrador inicio</t>
+  </si>
+  <si>
     <t>Procesamiento de la informacion</t>
   </si>
   <si>
@@ -74,6 +80,9 @@
   </si>
   <si>
     <t>Espiritu</t>
+  </si>
+  <si>
+    <t>Implementacion</t>
   </si>
 </sst>
 </file>
@@ -81,10 +90,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -97,9 +106,78 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -111,84 +189,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,15 +212,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -227,13 +243,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,12 +263,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -272,7 +335,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,7 +347,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,25 +377,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,78 +437,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -405,36 +444,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,26 +457,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -475,8 +486,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,49 +531,47 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -575,121 +584,121 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1015,10 +1024,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1052,12 +1061,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1065,7 +1085,7 @@
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1076,7 +1096,7 @@
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1087,15 +1107,15 @@
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -1106,7 +1126,7 @@
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1117,10 +1137,10 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1128,7 +1148,7 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1139,10 +1159,10 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>7</v>
@@ -1150,10 +1170,10 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -1161,10 +1181,15 @@
     </row>
     <row r="14" spans="2:3">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vision perspectiva-conclusion - borrador
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>cap</t>
   </si>
@@ -49,6 +49,9 @@
     <t>Estados de un proceso</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>Resolver un problema simple</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
   </si>
   <si>
     <t>Espiritu</t>
+  </si>
+  <si>
+    <t>Vision perspectiva - conclusion</t>
   </si>
   <si>
     <t>Implementacion</t>
@@ -90,9 +96,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -106,14 +112,44 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -121,7 +157,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,38 +172,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,6 +224,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -221,21 +241,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,19 +269,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,163 +359,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,28 +463,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,8 +475,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,6 +491,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -531,69 +535,68 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -602,103 +605,106 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1027,7 +1033,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1094,9 +1100,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1107,15 +1116,15 @@
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -1126,7 +1135,7 @@
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1137,7 +1146,7 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1148,7 +1157,7 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1159,7 +1168,7 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -1170,10 +1179,10 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -1181,15 +1190,26 @@
     </row>
     <row r="14" spans="2:3">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
otros ejemplos - borrador
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -96,10 +96,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -112,29 +112,60 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,44 +180,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -219,22 +212,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,181 +269,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,17 +460,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -486,23 +475,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,6 +491,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -537,174 +526,185 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1033,7 +1033,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1097,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">

</xml_diff>

<commit_message>
estados de un proceso
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -119,6 +119,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -127,6 +134,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -152,6 +167,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,6 +219,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -205,59 +235,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,187 +278,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,6 +469,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -520,32 +535,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -569,16 +558,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -593,127 +593,127 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1073,7 +1073,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -1101,7 +1101,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -1115,7 +1115,7 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -1132,7 +1132,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Wordpress version - capitulos 5 y 6
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>cap</t>
   </si>
@@ -31,51 +31,54 @@
     <t>Prologo</t>
   </si>
   <si>
+    <t>wordpress esp</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Idea general</t>
+  </si>
+  <si>
     <t>borrador parcial</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Idea general</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
     <t>Procesamiento de la informacion</t>
   </si>
   <si>
+    <t>Estados de un proceso</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Resolver un problema simple</t>
+  </si>
+  <si>
+    <t>Otros ejemplos de resolucion de problemas mas complejos</t>
+  </si>
+  <si>
+    <t>configuraciones</t>
+  </si>
+  <si>
+    <t>Eficiencia y numero de calculos</t>
+  </si>
+  <si>
+    <t>borrador final</t>
+  </si>
+  <si>
+    <t>Complejidad de un problema</t>
+  </si>
+  <si>
+    <t>Potencia del sistema</t>
+  </si>
+  <si>
     <t>borrador completo</t>
   </si>
   <si>
-    <t>Estados de un proceso</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Resolver un problema simple</t>
-  </si>
-  <si>
-    <t>Otros ejemplos de resolucion de problemas mas complejos</t>
-  </si>
-  <si>
-    <t>configuraciones</t>
-  </si>
-  <si>
-    <t>Eficiencia y numero de calculos</t>
-  </si>
-  <si>
-    <t>borrador final</t>
-  </si>
-  <si>
-    <t>Complejidad de un problema</t>
-  </si>
-  <si>
-    <t>Potencia del sistema</t>
-  </si>
-  <si>
     <t>Coste</t>
   </si>
   <si>
@@ -110,17 +113,41 @@
   </si>
   <si>
     <t>Chapter 3 - Resolver un problema</t>
+  </si>
+  <si>
+    <t>Chapter 4 - Caracteristicas</t>
+  </si>
+  <si>
+    <t>Chapter 5 - Eficiencia</t>
+  </si>
+  <si>
+    <t>Chapter 6 - Complejidad</t>
+  </si>
+  <si>
+    <t>Chapter 7 - Potencia</t>
+  </si>
+  <si>
+    <t>Chapter 8 - Costes</t>
+  </si>
+  <si>
+    <t>Chapter 9 - Redundancia</t>
+  </si>
+  <si>
+    <t>Chapter 10 - Configuraciones</t>
+  </si>
+  <si>
+    <t>Chapter 11 - Poda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -131,63 +158,50 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -199,39 +213,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,6 +246,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -247,29 +261,42 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,187 +317,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,39 +508,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -541,6 +535,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -552,6 +555,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,6 +591,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -584,13 +611,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -599,133 +626,133 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -735,52 +762,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
-    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
+    <cellStyle name="Coma" xfId="1" builtinId="3"/>
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
     <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
-    <cellStyle name="Coma" xfId="6" builtinId="3"/>
-    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21"/>
-    <cellStyle name="Nota" xfId="11" builtinId="10"/>
-    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
-    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
-    <cellStyle name="Título" xfId="14" builtinId="15"/>
-    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
-    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
-    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
-    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
-    <cellStyle name="Total" xfId="22" builtinId="25"/>
-    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
-    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
-    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
-    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
-    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
-    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
-    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
-    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
-    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
-    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
-    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
-    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
-    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
-    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
-    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
-    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
-    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
-    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
-    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
+    <cellStyle name="Moneda [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hipervínculo" xfId="6" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9"/>
+    <cellStyle name="Nota" xfId="8" builtinId="10"/>
+    <cellStyle name="Texto de advertencia" xfId="9" builtinId="11"/>
+    <cellStyle name="Título" xfId="10" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="11" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
+    <cellStyle name="Salida" xfId="17" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="19" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="22" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
+    <cellStyle name="Énfasis1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Énfasis1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Énfasis1" xfId="28" builtinId="32"/>
+    <cellStyle name="Énfasis2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="32" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="36" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="40" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Énfasis5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Énfasis5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Énfasis5" xfId="44" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Énfasis6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1051,10 +1078,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1096,21 +1123,21 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>7</v>
@@ -1141,7 +1168,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -1155,7 +1182,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -1166,7 +1193,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -1191,7 +1218,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -1205,7 +1232,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -1216,7 +1243,7 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1230,10 +1257,10 @@
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -1244,7 +1271,7 @@
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1258,18 +1285,18 @@
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -1277,12 +1304,15 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1290,7 +1320,10 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -1298,7 +1331,10 @@
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -1306,10 +1342,59 @@
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
       </c>
       <c r="D24">
         <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wordpress version - capitulo 8 esp
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>cap</t>
   </si>
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1372,14 +1372,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:2">
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="2:2">
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
       <c r="B29" t="s">
         <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:2">

</xml_diff>

<commit_message>
wordpress version - capitulo 9 esp
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>cap</t>
   </si>
@@ -144,10 +144,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -611,19 +611,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1388,9 +1388,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="2:3">
       <c r="B30" t="s">
         <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:2">

</xml_diff>

<commit_message>
wordpress version - capitulo 10 esp
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>cap</t>
   </si>
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1396,9 +1396,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:2">
+    <row r="31" spans="2:3">
       <c r="B31" t="s">
         <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:2">

</xml_diff>

<commit_message>
wordpress version - capitulo 11 esp
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12210"/>
+    <workbookView windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>cap</t>
   </si>
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1404,9 +1404,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:2">
+    <row r="32" spans="2:3">
       <c r="B32" t="s">
         <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
caps 0, 1 - esp - wordpress
</commit_message>
<xml_diff>
--- a/status plan.xlsx
+++ b/status plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t>cap</t>
   </si>
@@ -46,6 +46,9 @@
     <t>excerpt</t>
   </si>
   <si>
+    <t>review</t>
+  </si>
+  <si>
     <t>Prologo</t>
   </si>
   <si>
@@ -142,7 +145,13 @@
     <t>Chapter 6 - Complejidad</t>
   </si>
   <si>
+    <t>es  corto</t>
+  </si>
+  <si>
     <t>Chapter 7 - Potencia</t>
+  </si>
+  <si>
+    <t>es largo y necesita reestructurarse</t>
   </si>
   <si>
     <t>Chapter 8 - Costes</t>
@@ -1096,19 +1105,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="59.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="19.1428571428571" customWidth="1"/>
+    <col min="15" max="15" width="34.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:12">
+    <row r="1" s="1" customFormat="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1139,86 +1149,89 @@
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="2:5">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -1226,10 +1239,10 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -1237,102 +1250,102 @@
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -1340,15 +1353,15 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1356,13 +1369,16 @@
       <c r="K21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
       <c r="B22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -1370,13 +1386,16 @@
       <c r="K22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:11">
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
       <c r="B23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -1384,13 +1403,16 @@
       <c r="K23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:11">
+      <c r="N23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -1398,51 +1420,66 @@
       <c r="K24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:2">
+      <c r="N24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
       <c r="B25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11">
+        <v>40</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
       <c r="B26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:11">
+      <c r="N26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15">
       <c r="B27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:11">
+      <c r="O27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15">
       <c r="B28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K28">
         <v>1</v>
+      </c>
+      <c r="O28" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:11">
       <c r="B29" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -1450,10 +1487,10 @@
     </row>
     <row r="30" spans="2:11">
       <c r="B30" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -1461,10 +1498,10 @@
     </row>
     <row r="31" spans="2:11">
       <c r="B31" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -1472,10 +1509,10 @@
     </row>
     <row r="32" spans="2:11">
       <c r="B32" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K32">
         <v>1</v>

</xml_diff>